<commit_message>
added some excelplots and the QMQ Plot sourcecode
</commit_message>
<xml_diff>
--- a/Lech/RData/profiledata/Hoehenprofil_T2-T5.xlsx
+++ b/Lech/RData/profiledata/Hoehenprofil_T2-T5.xlsx
@@ -38,11 +38,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,6 +62,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -189,7 +195,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -268,6 +274,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -704,11 +711,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="58422117"/>
-        <c:axId val="46526946"/>
+        <c:axId val="3950276"/>
+        <c:axId val="43487184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58422117"/>
+        <c:axId val="3950276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -752,7 +759,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -774,12 +781,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46526946"/>
+        <c:crossAx val="43487184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46526946"/>
+        <c:axId val="43487184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="885"/>
@@ -824,7 +831,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -846,7 +853,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58422117"/>
+        <c:crossAx val="3950276"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -873,7 +880,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -940,6 +947,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -951,6 +959,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1273,11 +1282,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="4184135"/>
-        <c:axId val="37947576"/>
+        <c:axId val="40078388"/>
+        <c:axId val="51299687"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4184135"/>
+        <c:axId val="40078388"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -1321,7 +1330,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1343,12 +1352,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37947576"/>
+        <c:crossAx val="51299687"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37947576"/>
+        <c:axId val="51299687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="885"/>
@@ -1393,7 +1402,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1415,7 +1424,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4184135"/>
+        <c:crossAx val="40078388"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1442,7 +1451,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1521,6 +1530,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1831,11 +1841,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="93166190"/>
-        <c:axId val="98264272"/>
+        <c:axId val="67976341"/>
+        <c:axId val="99772584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93166190"/>
+        <c:axId val="67976341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -1879,7 +1889,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1901,12 +1911,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98264272"/>
+        <c:crossAx val="99772584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98264272"/>
+        <c:axId val="99772584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="885"/>
@@ -1951,7 +1961,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1973,7 +1983,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93166190"/>
+        <c:crossAx val="67976341"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2000,7 +2010,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2079,6 +2089,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2365,11 +2376,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65672907"/>
-        <c:axId val="37341518"/>
+        <c:axId val="32434380"/>
+        <c:axId val="14046523"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65672907"/>
+        <c:axId val="32434380"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -2413,7 +2424,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2435,12 +2446,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37341518"/>
+        <c:crossAx val="14046523"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37341518"/>
+        <c:axId val="14046523"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="885"/>
@@ -2485,7 +2496,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2507,7 +2518,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65672907"/>
+        <c:crossAx val="32434380"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2545,9 +2556,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
+      <xdr:colOff>66240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2556,7 +2567,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3165480" y="319680"/>
-        <a:ext cx="5761800" cy="3241800"/>
+        <a:ext cx="5761440" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2580,9 +2591,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>72720</xdr:colOff>
+      <xdr:colOff>72360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2591,7 +2602,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3171600" y="325440"/>
-        <a:ext cx="5761800" cy="3241800"/>
+        <a:ext cx="5761440" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2615,9 +2626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>75240</xdr:colOff>
+      <xdr:colOff>74880</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2625,8 +2636,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3164400" y="323640"/>
-        <a:ext cx="5761800" cy="3241800"/>
+        <a:off x="3165120" y="323640"/>
+        <a:ext cx="5761440" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2645,14 +2656,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>810000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>69480</xdr:colOff>
+      <xdr:colOff>69120</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2660,8 +2671,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3288960" y="327240"/>
-        <a:ext cx="5761800" cy="3241800"/>
+        <a:off x="3290040" y="318960"/>
+        <a:ext cx="5761440" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3263,7 +3274,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3675,7 +3686,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
@@ -3697,7 +3708,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
@@ -4089,7 +4100,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
@@ -4111,7 +4122,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -4470,7 +4481,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>